<commit_message>
REFACTOR - Mudancas no estilo geral e fixes
</commit_message>
<xml_diff>
--- a/DOCS/burn_sprint2.xlsx
+++ b/DOCS/burn_sprint2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\FATEC\sem2\API-2\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FD78575-40D7-4139-ADBD-1D8B9C997396}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3C6E831-5538-4735-B6CB-DD2BDB71F05A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>Total de horas</t>
   </si>
@@ -123,9 +123,6 @@
     <t>S7 - Daniel</t>
   </si>
   <si>
-    <t>S0 - Git e docs (Matesco)</t>
-  </si>
-  <si>
     <t>S2.1 - Front</t>
   </si>
   <si>
@@ -151,6 +148,21 @@
   </si>
   <si>
     <t>S4 - Estudo</t>
+  </si>
+  <si>
+    <t>S8.1 - Rafael</t>
+  </si>
+  <si>
+    <t>S8.2 - Rafael</t>
+  </si>
+  <si>
+    <t>S8.3 - Rafael</t>
+  </si>
+  <si>
+    <t>S9 - Rafael</t>
+  </si>
+  <si>
+    <t>S0 - Git e docs</t>
   </si>
 </sst>
 </file>
@@ -183,7 +195,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -200,6 +212,12 @@
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -267,7 +285,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -285,6 +303,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -904,67 +925,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>96</c:v>
+                  <c:v>104</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>96</c:v>
+                  <c:v>103</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>91.5</c:v>
+                  <c:v>98.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>90.5</c:v>
+                  <c:v>97.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>89.5</c:v>
+                  <c:v>92.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>89.5</c:v>
+                  <c:v>87.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>89.5</c:v>
+                  <c:v>85.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>89.5</c:v>
+                  <c:v>82.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>89.5</c:v>
+                  <c:v>77.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>89.5</c:v>
+                  <c:v>70.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>89.5</c:v>
+                  <c:v>64.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>89.5</c:v>
+                  <c:v>63.5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>89.5</c:v>
+                  <c:v>63.5</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>89.5</c:v>
+                  <c:v>63.5</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>89.5</c:v>
+                  <c:v>63.5</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>89.5</c:v>
+                  <c:v>63.5</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>89.5</c:v>
+                  <c:v>63.5</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>89.5</c:v>
+                  <c:v>63.5</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>89.5</c:v>
+                  <c:v>63.5</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>89.5</c:v>
+                  <c:v>63.5</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>89.5</c:v>
+                  <c:v>63.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1078,64 +1099,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>96</c:v>
+                  <c:v>104</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>91.2</c:v>
+                  <c:v>98.8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>86.4</c:v>
+                  <c:v>93.6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>81.599999999999994</c:v>
+                  <c:v>88.4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>76.8</c:v>
+                  <c:v>83.2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>72</c:v>
+                  <c:v>78</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>67.2</c:v>
+                  <c:v>72.8</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>67.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>62.4</c:v>
                 </c:pt>
-                <c:pt idx="8">
-                  <c:v>57.6</c:v>
-                </c:pt>
                 <c:pt idx="9">
-                  <c:v>52.800000000000004</c:v>
+                  <c:v>57.199999999999996</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>48</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43.2</c:v>
+                  <c:v>46.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>38.400000000000006</c:v>
+                  <c:v>41.599999999999994</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>33.6</c:v>
+                  <c:v>36.399999999999991</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>28.799999999999997</c:v>
+                  <c:v>31.200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>24</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>19.200000000000003</c:v>
+                  <c:v>20.799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>14.400000000000006</c:v>
+                  <c:v>15.599999999999994</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>9.6000000000000085</c:v>
+                  <c:v>10.399999999999991</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4.7999999999999972</c:v>
+                  <c:v>5.2000000000000028</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>0</c:v>
@@ -1547,67 +1568,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>96</c:v>
+                  <c:v>104</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>96</c:v>
+                  <c:v>103</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>91.5</c:v>
+                  <c:v>98.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>90.5</c:v>
+                  <c:v>97.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>89.5</c:v>
+                  <c:v>92.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>89.5</c:v>
+                  <c:v>87.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>89.5</c:v>
+                  <c:v>85.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>89.5</c:v>
+                  <c:v>82.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>89.5</c:v>
+                  <c:v>77.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>89.5</c:v>
+                  <c:v>70.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>89.5</c:v>
+                  <c:v>64.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>89.5</c:v>
+                  <c:v>63.5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>89.5</c:v>
+                  <c:v>63.5</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>89.5</c:v>
+                  <c:v>63.5</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>89.5</c:v>
+                  <c:v>63.5</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>89.5</c:v>
+                  <c:v>63.5</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>89.5</c:v>
+                  <c:v>63.5</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>89.5</c:v>
+                  <c:v>63.5</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>89.5</c:v>
+                  <c:v>63.5</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>89.5</c:v>
+                  <c:v>63.5</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>89.5</c:v>
+                  <c:v>63.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1721,64 +1742,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>96</c:v>
+                  <c:v>104</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>91.2</c:v>
+                  <c:v>98.8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>86.4</c:v>
+                  <c:v>93.6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>81.599999999999994</c:v>
+                  <c:v>88.4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>76.8</c:v>
+                  <c:v>83.2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>72</c:v>
+                  <c:v>78</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>67.2</c:v>
+                  <c:v>72.8</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>67.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>62.4</c:v>
                 </c:pt>
-                <c:pt idx="8">
-                  <c:v>57.6</c:v>
-                </c:pt>
                 <c:pt idx="9">
-                  <c:v>52.800000000000004</c:v>
+                  <c:v>57.199999999999996</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>48</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43.2</c:v>
+                  <c:v>46.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>38.400000000000006</c:v>
+                  <c:v>41.599999999999994</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>33.6</c:v>
+                  <c:v>36.399999999999991</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>28.799999999999997</c:v>
+                  <c:v>31.200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>24</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>19.200000000000003</c:v>
+                  <c:v>20.799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>14.400000000000006</c:v>
+                  <c:v>15.599999999999994</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>9.6000000000000085</c:v>
+                  <c:v>10.399999999999991</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4.7999999999999972</c:v>
+                  <c:v>5.2000000000000028</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>0</c:v>
@@ -2415,8 +2436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AD35" sqref="AD35"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2462,7 +2483,7 @@
       <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="7" t="s">
         <v>10</v>
       </c>
       <c r="M1" s="1" t="s">
@@ -2511,8 +2532,12 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
+      <c r="K2" s="1">
+        <v>1</v>
+      </c>
+      <c r="L2" s="1">
+        <v>2</v>
+      </c>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
@@ -2526,7 +2551,7 @@
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" s="1">
         <v>3</v>
@@ -2538,9 +2563,13 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
+      <c r="J3" s="1">
+        <v>1</v>
+      </c>
       <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
+      <c r="L3" s="1">
+        <v>1</v>
+      </c>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
@@ -2554,7 +2583,7 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4" s="1">
         <v>3</v>
@@ -2582,7 +2611,7 @@
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" s="1">
         <v>3</v>
@@ -2610,7 +2639,7 @@
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B6" s="1">
         <v>8</v>
@@ -2619,12 +2648,18 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
+      <c r="G6" s="1">
+        <v>1</v>
+      </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
+      <c r="J6" s="1">
+        <v>4</v>
+      </c>
       <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
+      <c r="L6" s="1">
+        <v>1</v>
+      </c>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
@@ -2638,7 +2673,7 @@
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B7" s="1">
         <v>8</v>
@@ -2666,7 +2701,7 @@
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B8" s="1">
         <v>5</v>
@@ -2707,7 +2742,9 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
+      <c r="K9" s="1">
+        <v>2</v>
+      </c>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
@@ -2725,7 +2762,7 @@
         <v>27</v>
       </c>
       <c r="B10" s="1">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -2735,8 +2772,12 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
+      <c r="K10" s="1">
+        <v>4</v>
+      </c>
+      <c r="L10" s="1">
+        <v>2</v>
+      </c>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
@@ -2805,12 +2846,18 @@
       <c r="V12" s="1"/>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
+      <c r="A13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1</v>
+      </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
+      <c r="F13" s="1">
+        <v>1</v>
+      </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
@@ -2829,12 +2876,18 @@
       <c r="V13" s="1"/>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="1"/>
+      <c r="A14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1</v>
+      </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
+      <c r="F14" s="1">
+        <v>1</v>
+      </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
@@ -2853,13 +2906,21 @@
       <c r="V14" s="1"/>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="1"/>
+      <c r="A15" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="1">
+        <v>3</v>
+      </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
+      <c r="F15" s="1">
+        <v>1</v>
+      </c>
+      <c r="G15" s="1">
+        <v>2</v>
+      </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
@@ -2877,15 +2938,23 @@
       <c r="V15" s="1"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
+      <c r="A16" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="1">
+        <v>8</v>
+      </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
+      <c r="H16" s="1">
+        <v>2</v>
+      </c>
+      <c r="I16" s="1">
+        <v>3</v>
+      </c>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
@@ -2998,7 +3067,7 @@
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B21" s="1">
         <v>5</v>
@@ -3028,7 +3097,7 @@
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B22" s="1">
         <v>3</v>
@@ -3036,8 +3105,12 @@
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
+      <c r="F22" s="1">
+        <v>1</v>
+      </c>
+      <c r="G22" s="1">
+        <v>2</v>
+      </c>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
@@ -3056,7 +3129,7 @@
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B23" s="1">
         <v>8</v>
@@ -3086,12 +3159,14 @@
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="B24" s="1">
         <v>8</v>
       </c>
-      <c r="C24" s="1"/>
+      <c r="C24" s="1">
+        <v>1</v>
+      </c>
       <c r="D24" s="1">
         <v>1</v>
       </c>
@@ -3107,7 +3182,9 @@
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
+      <c r="M24" s="1">
+        <v>1</v>
+      </c>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
@@ -3124,87 +3201,87 @@
       </c>
       <c r="B25" s="4">
         <f>SUM(B2:B24)</f>
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="C25" s="4">
         <f t="shared" ref="C25:V25" si="0">B25-SUM(C2:C24)</f>
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="D25" s="4">
         <f t="shared" si="0"/>
-        <v>91.5</v>
+        <v>98.5</v>
       </c>
       <c r="E25" s="4">
         <f t="shared" si="0"/>
-        <v>90.5</v>
+        <v>97.5</v>
       </c>
       <c r="F25" s="4">
         <f t="shared" si="0"/>
-        <v>89.5</v>
+        <v>92.5</v>
       </c>
       <c r="G25" s="4">
         <f t="shared" si="0"/>
-        <v>89.5</v>
+        <v>87.5</v>
       </c>
       <c r="H25" s="4">
         <f t="shared" si="0"/>
-        <v>89.5</v>
+        <v>85.5</v>
       </c>
       <c r="I25" s="4">
         <f t="shared" si="0"/>
-        <v>89.5</v>
+        <v>82.5</v>
       </c>
       <c r="J25" s="4">
         <f t="shared" si="0"/>
-        <v>89.5</v>
+        <v>77.5</v>
       </c>
       <c r="K25" s="4">
         <f t="shared" si="0"/>
-        <v>89.5</v>
+        <v>70.5</v>
       </c>
       <c r="L25" s="4">
         <f t="shared" si="0"/>
-        <v>89.5</v>
+        <v>64.5</v>
       </c>
       <c r="M25" s="4">
         <f t="shared" si="0"/>
-        <v>89.5</v>
+        <v>63.5</v>
       </c>
       <c r="N25" s="4">
         <f t="shared" si="0"/>
-        <v>89.5</v>
+        <v>63.5</v>
       </c>
       <c r="O25" s="4">
         <f t="shared" si="0"/>
-        <v>89.5</v>
+        <v>63.5</v>
       </c>
       <c r="P25" s="4">
         <f t="shared" si="0"/>
-        <v>89.5</v>
+        <v>63.5</v>
       </c>
       <c r="Q25" s="4">
         <f t="shared" si="0"/>
-        <v>89.5</v>
+        <v>63.5</v>
       </c>
       <c r="R25" s="4">
         <f t="shared" si="0"/>
-        <v>89.5</v>
+        <v>63.5</v>
       </c>
       <c r="S25" s="4">
         <f t="shared" si="0"/>
-        <v>89.5</v>
+        <v>63.5</v>
       </c>
       <c r="T25" s="4">
         <f t="shared" si="0"/>
-        <v>89.5</v>
+        <v>63.5</v>
       </c>
       <c r="U25" s="4">
         <f t="shared" si="0"/>
-        <v>89.5</v>
+        <v>63.5</v>
       </c>
       <c r="V25" s="4">
         <f t="shared" si="0"/>
-        <v>89.5</v>
+        <v>63.5</v>
       </c>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
@@ -3212,83 +3289,83 @@
         <v>22</v>
       </c>
       <c r="B26" s="6">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="C26" s="6">
         <f>$B$26-(($B$26/20)*(COLUMN()-2))</f>
-        <v>91.2</v>
+        <v>98.8</v>
       </c>
       <c r="D26" s="6">
         <f t="shared" ref="D26:V26" si="1">$B$26-(($B$26/20)*(COLUMN()-2))</f>
-        <v>86.4</v>
+        <v>93.6</v>
       </c>
       <c r="E26" s="6">
         <f t="shared" si="1"/>
-        <v>81.599999999999994</v>
+        <v>88.4</v>
       </c>
       <c r="F26" s="6">
         <f t="shared" si="1"/>
-        <v>76.8</v>
+        <v>83.2</v>
       </c>
       <c r="G26" s="6">
         <f t="shared" si="1"/>
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="H26" s="6">
         <f t="shared" si="1"/>
-        <v>67.2</v>
+        <v>72.8</v>
       </c>
       <c r="I26" s="6">
         <f t="shared" si="1"/>
-        <v>62.4</v>
+        <v>67.599999999999994</v>
       </c>
       <c r="J26" s="6">
         <f t="shared" si="1"/>
-        <v>57.6</v>
+        <v>62.4</v>
       </c>
       <c r="K26" s="6">
         <f t="shared" si="1"/>
-        <v>52.800000000000004</v>
+        <v>57.199999999999996</v>
       </c>
       <c r="L26" s="6">
         <f t="shared" si="1"/>
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="M26" s="6">
         <f t="shared" si="1"/>
-        <v>43.2</v>
+        <v>46.8</v>
       </c>
       <c r="N26" s="6">
         <f t="shared" si="1"/>
-        <v>38.400000000000006</v>
+        <v>41.599999999999994</v>
       </c>
       <c r="O26" s="6">
         <f t="shared" si="1"/>
-        <v>33.6</v>
+        <v>36.399999999999991</v>
       </c>
       <c r="P26" s="6">
         <f t="shared" si="1"/>
-        <v>28.799999999999997</v>
+        <v>31.200000000000003</v>
       </c>
       <c r="Q26" s="6">
         <f t="shared" si="1"/>
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="R26" s="6">
         <f t="shared" si="1"/>
-        <v>19.200000000000003</v>
+        <v>20.799999999999997</v>
       </c>
       <c r="S26" s="6">
         <f t="shared" si="1"/>
-        <v>14.400000000000006</v>
+        <v>15.599999999999994</v>
       </c>
       <c r="T26" s="6">
         <f t="shared" si="1"/>
-        <v>9.6000000000000085</v>
+        <v>10.399999999999991</v>
       </c>
       <c r="U26" s="6">
         <f t="shared" si="1"/>
-        <v>4.7999999999999972</v>
+        <v>5.2000000000000028</v>
       </c>
       <c r="V26" s="6">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
FEAT - Atualiza lógica de inserção de usuário e ajusta visibilidade de botões no layout
</commit_message>
<xml_diff>
--- a/DOCS/burn_sprint2.xlsx
+++ b/DOCS/burn_sprint2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\FATEC\sem2\API-2\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3C6E831-5538-4735-B6CB-DD2BDB71F05A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E447C590-9DC0-4D76-A09A-6ECC9DC9A69E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -925,67 +925,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>104</c:v>
+                  <c:v>106</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>103</c:v>
+                  <c:v>105</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>98.5</c:v>
+                  <c:v>100.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>97.5</c:v>
+                  <c:v>96.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>92.5</c:v>
+                  <c:v>91.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>87.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>85.5</c:v>
+                  <c:v>84.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>82.5</c:v>
+                  <c:v>79.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>77.5</c:v>
+                  <c:v>74.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>70.5</c:v>
+                  <c:v>72.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>64.5</c:v>
+                  <c:v>62.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>63.5</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>63.5</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>63.5</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>63.5</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>63.5</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>63.5</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>63.5</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>63.5</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>63.5</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>63.5</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1099,64 +1099,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>104</c:v>
+                  <c:v>106</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>98.8</c:v>
+                  <c:v>100.7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>93.6</c:v>
+                  <c:v>95.4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>88.4</c:v>
+                  <c:v>90.1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>83.2</c:v>
+                  <c:v>84.8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>78</c:v>
+                  <c:v>79.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>72.8</c:v>
+                  <c:v>74.2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>67.599999999999994</c:v>
+                  <c:v>68.900000000000006</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>62.4</c:v>
+                  <c:v>63.6</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>57.199999999999996</c:v>
+                  <c:v>58.300000000000004</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>52</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>46.8</c:v>
+                  <c:v>47.7</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>41.599999999999994</c:v>
+                  <c:v>42.400000000000006</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>36.399999999999991</c:v>
+                  <c:v>37.100000000000009</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>31.200000000000003</c:v>
+                  <c:v>31.799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>26</c:v>
+                  <c:v>26.5</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>20.799999999999997</c:v>
+                  <c:v>21.200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>15.599999999999994</c:v>
+                  <c:v>15.900000000000006</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>10.399999999999991</c:v>
+                  <c:v>10.600000000000009</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5.2000000000000028</c:v>
+                  <c:v>5.2999999999999972</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>0</c:v>
@@ -1568,67 +1568,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>104</c:v>
+                  <c:v>106</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>103</c:v>
+                  <c:v>105</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>98.5</c:v>
+                  <c:v>100.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>97.5</c:v>
+                  <c:v>96.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>92.5</c:v>
+                  <c:v>91.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>87.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>85.5</c:v>
+                  <c:v>84.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>82.5</c:v>
+                  <c:v>79.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>77.5</c:v>
+                  <c:v>74.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>70.5</c:v>
+                  <c:v>72.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>64.5</c:v>
+                  <c:v>62.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>63.5</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>63.5</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>63.5</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>63.5</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>63.5</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>63.5</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>63.5</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>63.5</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>63.5</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>63.5</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1742,64 +1742,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>104</c:v>
+                  <c:v>106</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>98.8</c:v>
+                  <c:v>100.7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>93.6</c:v>
+                  <c:v>95.4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>88.4</c:v>
+                  <c:v>90.1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>83.2</c:v>
+                  <c:v>84.8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>78</c:v>
+                  <c:v>79.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>72.8</c:v>
+                  <c:v>74.2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>67.599999999999994</c:v>
+                  <c:v>68.900000000000006</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>62.4</c:v>
+                  <c:v>63.6</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>57.199999999999996</c:v>
+                  <c:v>58.300000000000004</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>52</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>46.8</c:v>
+                  <c:v>47.7</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>41.599999999999994</c:v>
+                  <c:v>42.400000000000006</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>36.399999999999991</c:v>
+                  <c:v>37.100000000000009</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>31.200000000000003</c:v>
+                  <c:v>31.799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>26</c:v>
+                  <c:v>26.5</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>20.799999999999997</c:v>
+                  <c:v>21.200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>15.599999999999994</c:v>
+                  <c:v>15.900000000000006</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>10.399999999999991</c:v>
+                  <c:v>10.600000000000009</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5.2000000000000028</c:v>
+                  <c:v>5.2999999999999972</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>0</c:v>
@@ -2437,7 +2437,7 @@
   <dimension ref="A1:V26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2531,14 +2531,16 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1">
+      <c r="J2" s="1">
         <v>1</v>
       </c>
+      <c r="K2" s="1"/>
       <c r="L2" s="1">
         <v>2</v>
       </c>
-      <c r="M2" s="1"/>
+      <c r="M2" s="1">
+        <v>3</v>
+      </c>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
@@ -2562,10 +2564,10 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1">
+      <c r="I3" s="1">
         <v>1</v>
       </c>
+      <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1">
         <v>1</v>
@@ -2598,7 +2600,9 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
+      <c r="M4" s="1">
+        <v>1.5</v>
+      </c>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
@@ -2647,15 +2651,15 @@
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1">
+      <c r="F6" s="1">
         <v>1</v>
       </c>
+      <c r="G6" s="1"/>
       <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1">
+      <c r="I6" s="1">
         <v>4</v>
       </c>
+      <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1">
         <v>1</v>
@@ -2771,10 +2775,10 @@
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1">
+      <c r="J10" s="1">
         <v>4</v>
       </c>
+      <c r="K10" s="1"/>
       <c r="L10" s="1">
         <v>2</v>
       </c>
@@ -2854,10 +2858,10 @@
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1">
+      <c r="E13" s="1">
         <v>1</v>
       </c>
+      <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
@@ -2884,10 +2888,10 @@
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1">
+      <c r="E14" s="1">
         <v>1</v>
       </c>
+      <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
@@ -2914,13 +2918,13 @@
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
+      <c r="E15" s="1">
+        <v>1</v>
+      </c>
       <c r="F15" s="1">
-        <v>1</v>
-      </c>
-      <c r="G15" s="1">
         <v>2</v>
       </c>
+      <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
@@ -2942,23 +2946,27 @@
         <v>41</v>
       </c>
       <c r="B16" s="1">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
+      <c r="G16" s="1">
+        <v>2</v>
+      </c>
       <c r="H16" s="1">
-        <v>2</v>
-      </c>
-      <c r="I16" s="1">
         <v>3</v>
       </c>
+      <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
+      <c r="L16" s="1">
+        <v>2</v>
+      </c>
+      <c r="M16" s="1">
+        <v>4</v>
+      </c>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
@@ -3132,7 +3140,7 @@
         <v>32</v>
       </c>
       <c r="B23" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1">
@@ -3145,7 +3153,9 @@
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
+      <c r="L23" s="1">
+        <v>1</v>
+      </c>
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
@@ -3181,10 +3191,10 @@
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-      <c r="M24" s="1">
+      <c r="L24" s="1">
         <v>1</v>
       </c>
+      <c r="M24" s="1"/>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
@@ -3201,23 +3211,23 @@
       </c>
       <c r="B25" s="4">
         <f>SUM(B2:B24)</f>
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C25" s="4">
         <f t="shared" ref="C25:V25" si="0">B25-SUM(C2:C24)</f>
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D25" s="4">
         <f t="shared" si="0"/>
-        <v>98.5</v>
+        <v>100.5</v>
       </c>
       <c r="E25" s="4">
         <f t="shared" si="0"/>
-        <v>97.5</v>
+        <v>96.5</v>
       </c>
       <c r="F25" s="4">
         <f t="shared" si="0"/>
-        <v>92.5</v>
+        <v>91.5</v>
       </c>
       <c r="G25" s="4">
         <f t="shared" si="0"/>
@@ -3225,63 +3235,63 @@
       </c>
       <c r="H25" s="4">
         <f t="shared" si="0"/>
-        <v>85.5</v>
+        <v>84.5</v>
       </c>
       <c r="I25" s="4">
-        <f t="shared" si="0"/>
-        <v>82.5</v>
+        <f>H25-SUM(I2:I24)</f>
+        <v>79.5</v>
       </c>
       <c r="J25" s="4">
         <f t="shared" si="0"/>
-        <v>77.5</v>
+        <v>74.5</v>
       </c>
       <c r="K25" s="4">
         <f t="shared" si="0"/>
-        <v>70.5</v>
+        <v>72.5</v>
       </c>
       <c r="L25" s="4">
-        <f t="shared" si="0"/>
-        <v>64.5</v>
+        <f>K25-SUM(L2:L24)</f>
+        <v>62.5</v>
       </c>
       <c r="M25" s="4">
         <f t="shared" si="0"/>
-        <v>63.5</v>
+        <v>54</v>
       </c>
       <c r="N25" s="4">
         <f t="shared" si="0"/>
-        <v>63.5</v>
+        <v>54</v>
       </c>
       <c r="O25" s="4">
         <f t="shared" si="0"/>
-        <v>63.5</v>
+        <v>54</v>
       </c>
       <c r="P25" s="4">
         <f t="shared" si="0"/>
-        <v>63.5</v>
+        <v>54</v>
       </c>
       <c r="Q25" s="4">
         <f t="shared" si="0"/>
-        <v>63.5</v>
+        <v>54</v>
       </c>
       <c r="R25" s="4">
         <f t="shared" si="0"/>
-        <v>63.5</v>
+        <v>54</v>
       </c>
       <c r="S25" s="4">
         <f t="shared" si="0"/>
-        <v>63.5</v>
+        <v>54</v>
       </c>
       <c r="T25" s="4">
         <f t="shared" si="0"/>
-        <v>63.5</v>
+        <v>54</v>
       </c>
       <c r="U25" s="4">
         <f t="shared" si="0"/>
-        <v>63.5</v>
+        <v>54</v>
       </c>
       <c r="V25" s="4">
         <f t="shared" si="0"/>
-        <v>63.5</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
@@ -3289,83 +3299,83 @@
         <v>22</v>
       </c>
       <c r="B26" s="6">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C26" s="6">
         <f>$B$26-(($B$26/20)*(COLUMN()-2))</f>
-        <v>98.8</v>
+        <v>100.7</v>
       </c>
       <c r="D26" s="6">
         <f t="shared" ref="D26:V26" si="1">$B$26-(($B$26/20)*(COLUMN()-2))</f>
-        <v>93.6</v>
+        <v>95.4</v>
       </c>
       <c r="E26" s="6">
         <f t="shared" si="1"/>
-        <v>88.4</v>
+        <v>90.1</v>
       </c>
       <c r="F26" s="6">
         <f t="shared" si="1"/>
-        <v>83.2</v>
+        <v>84.8</v>
       </c>
       <c r="G26" s="6">
         <f t="shared" si="1"/>
-        <v>78</v>
+        <v>79.5</v>
       </c>
       <c r="H26" s="6">
         <f t="shared" si="1"/>
-        <v>72.8</v>
+        <v>74.2</v>
       </c>
       <c r="I26" s="6">
         <f t="shared" si="1"/>
-        <v>67.599999999999994</v>
+        <v>68.900000000000006</v>
       </c>
       <c r="J26" s="6">
         <f t="shared" si="1"/>
-        <v>62.4</v>
+        <v>63.6</v>
       </c>
       <c r="K26" s="6">
         <f t="shared" si="1"/>
-        <v>57.199999999999996</v>
+        <v>58.300000000000004</v>
       </c>
       <c r="L26" s="6">
         <f t="shared" si="1"/>
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="M26" s="6">
         <f t="shared" si="1"/>
-        <v>46.8</v>
+        <v>47.7</v>
       </c>
       <c r="N26" s="6">
         <f t="shared" si="1"/>
-        <v>41.599999999999994</v>
+        <v>42.400000000000006</v>
       </c>
       <c r="O26" s="6">
         <f t="shared" si="1"/>
-        <v>36.399999999999991</v>
+        <v>37.100000000000009</v>
       </c>
       <c r="P26" s="6">
         <f t="shared" si="1"/>
-        <v>31.200000000000003</v>
+        <v>31.799999999999997</v>
       </c>
       <c r="Q26" s="6">
         <f t="shared" si="1"/>
-        <v>26</v>
+        <v>26.5</v>
       </c>
       <c r="R26" s="6">
         <f t="shared" si="1"/>
-        <v>20.799999999999997</v>
+        <v>21.200000000000003</v>
       </c>
       <c r="S26" s="6">
         <f t="shared" si="1"/>
-        <v>15.599999999999994</v>
+        <v>15.900000000000006</v>
       </c>
       <c r="T26" s="6">
         <f t="shared" si="1"/>
-        <v>10.399999999999991</v>
+        <v>10.600000000000009</v>
       </c>
       <c r="U26" s="6">
         <f t="shared" si="1"/>
-        <v>5.2000000000000028</v>
+        <v>5.2999999999999972</v>
       </c>
       <c r="V26" s="6">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
DOCS - Burndown sprint 2 atualizado
</commit_message>
<xml_diff>
--- a/DOCS/burn_sprint2.xlsx
+++ b/DOCS/burn_sprint2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\FATEC\sem2\API-2\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3C6E831-5538-4735-B6CB-DD2BDB71F05A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ABA6FB2-00A5-4A41-BD02-5B24E4939F42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Burndown Chart" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>Total de horas</t>
   </si>
@@ -111,9 +111,6 @@
     <t>S1 - Daniel</t>
   </si>
   <si>
-    <t>S4 - Caio</t>
-  </si>
-  <si>
     <t>S6 - Monteiro</t>
   </si>
   <si>
@@ -163,6 +160,18 @@
   </si>
   <si>
     <t>S0 - Git e docs</t>
+  </si>
+  <si>
+    <t>S4 - Matesco</t>
+  </si>
+  <si>
+    <t>S10 - Front</t>
+  </si>
+  <si>
+    <t>S11 - Caio</t>
+  </si>
+  <si>
+    <t>S12 - Front</t>
   </si>
 </sst>
 </file>
@@ -925,67 +934,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>104</c:v>
+                  <c:v>110</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>103</c:v>
+                  <c:v>109</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>104.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>103.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>98.5</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>97.5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>92.5</c:v>
-                </c:pt>
                 <c:pt idx="5">
-                  <c:v>87.5</c:v>
+                  <c:v>93.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>85.5</c:v>
+                  <c:v>91.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>82.5</c:v>
+                  <c:v>88.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>77.5</c:v>
+                  <c:v>81.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>70.5</c:v>
+                  <c:v>74.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>64.5</c:v>
+                  <c:v>66.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>63.5</c:v>
+                  <c:v>55.5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>63.5</c:v>
+                  <c:v>45.5</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>63.5</c:v>
+                  <c:v>43.5</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>63.5</c:v>
+                  <c:v>37.5</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>63.5</c:v>
+                  <c:v>32.5</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>63.5</c:v>
+                  <c:v>32.5</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>63.5</c:v>
+                  <c:v>32.5</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>63.5</c:v>
+                  <c:v>32.5</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>63.5</c:v>
+                  <c:v>32.5</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>63.5</c:v>
+                  <c:v>32.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1099,64 +1108,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>104</c:v>
+                  <c:v>110</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>98.8</c:v>
+                  <c:v>104.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>93.6</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>88.4</c:v>
+                  <c:v>93.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>83.2</c:v>
+                  <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>78</c:v>
+                  <c:v>82.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>72.8</c:v>
+                  <c:v>77</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>67.599999999999994</c:v>
+                  <c:v>71.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>62.4</c:v>
+                  <c:v>66</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>57.199999999999996</c:v>
+                  <c:v>60.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>52</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>46.8</c:v>
+                  <c:v>49.5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>41.599999999999994</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>36.399999999999991</c:v>
+                  <c:v>38.5</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>31.200000000000003</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>26</c:v>
+                  <c:v>27.5</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>20.799999999999997</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>15.599999999999994</c:v>
+                  <c:v>16.5</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>10.399999999999991</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5.2000000000000028</c:v>
+                  <c:v>5.5</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>0</c:v>
@@ -1335,6 +1344,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.35927896675045001"/>
+          <c:y val="0.9466793453556962"/>
+          <c:w val="0.27740086405363151"/>
+          <c:h val="5.3320654644303807E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1568,67 +1587,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>104</c:v>
+                  <c:v>110</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>103</c:v>
+                  <c:v>109</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>104.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>103.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>98.5</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>97.5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>92.5</c:v>
-                </c:pt>
                 <c:pt idx="5">
-                  <c:v>87.5</c:v>
+                  <c:v>93.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>85.5</c:v>
+                  <c:v>91.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>82.5</c:v>
+                  <c:v>88.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>77.5</c:v>
+                  <c:v>81.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>70.5</c:v>
+                  <c:v>74.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>64.5</c:v>
+                  <c:v>66.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>63.5</c:v>
+                  <c:v>55.5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>63.5</c:v>
+                  <c:v>45.5</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>63.5</c:v>
+                  <c:v>43.5</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>63.5</c:v>
+                  <c:v>37.5</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>63.5</c:v>
+                  <c:v>32.5</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>63.5</c:v>
+                  <c:v>32.5</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>63.5</c:v>
+                  <c:v>32.5</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>63.5</c:v>
+                  <c:v>32.5</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>63.5</c:v>
+                  <c:v>32.5</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>63.5</c:v>
+                  <c:v>32.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1742,64 +1761,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>104</c:v>
+                  <c:v>110</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>98.8</c:v>
+                  <c:v>104.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>93.6</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>88.4</c:v>
+                  <c:v>93.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>83.2</c:v>
+                  <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>78</c:v>
+                  <c:v>82.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>72.8</c:v>
+                  <c:v>77</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>67.599999999999994</c:v>
+                  <c:v>71.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>62.4</c:v>
+                  <c:v>66</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>57.199999999999996</c:v>
+                  <c:v>60.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>52</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>46.8</c:v>
+                  <c:v>49.5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>41.599999999999994</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>36.399999999999991</c:v>
+                  <c:v>38.5</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>31.200000000000003</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>26</c:v>
+                  <c:v>27.5</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>20.799999999999997</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>15.599999999999994</c:v>
+                  <c:v>16.5</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>10.399999999999991</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5.2000000000000028</c:v>
+                  <c:v>5.5</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>0</c:v>
@@ -2049,11 +2068,11 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>390524</xdr:colOff>
+      <xdr:colOff>390525</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>14287</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="6191250" cy="3638551"/>
+    <xdr:ext cx="5514976" cy="4019343"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -2436,8 +2455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AH17" sqref="AH17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2539,7 +2558,9 @@
         <v>2</v>
       </c>
       <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
+      <c r="N2" s="1">
+        <v>3</v>
+      </c>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
@@ -2551,7 +2572,7 @@
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3" s="1">
         <v>3</v>
@@ -2571,7 +2592,9 @@
         <v>1</v>
       </c>
       <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
+      <c r="N3" s="1">
+        <v>1</v>
+      </c>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
@@ -2583,7 +2606,7 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" s="1">
         <v>3</v>
@@ -2598,8 +2621,12 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
+      <c r="M4" s="1">
+        <v>2</v>
+      </c>
+      <c r="N4" s="1">
+        <v>1</v>
+      </c>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
@@ -2611,7 +2638,7 @@
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" s="1">
         <v>3</v>
@@ -2626,7 +2653,9 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
+      <c r="M5" s="1">
+        <v>1</v>
+      </c>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
@@ -2639,7 +2668,7 @@
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B6" s="1">
         <v>8</v>
@@ -2660,10 +2689,16 @@
       <c r="L6" s="1">
         <v>1</v>
       </c>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
+      <c r="M6" s="1">
+        <v>2</v>
+      </c>
+      <c r="N6" s="1">
+        <v>1</v>
+      </c>
       <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
+      <c r="P6" s="1">
+        <v>1</v>
+      </c>
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
@@ -2673,7 +2708,7 @@
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B7" s="1">
         <v>8</v>
@@ -2685,7 +2720,9 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
+      <c r="J7" s="1">
+        <v>2</v>
+      </c>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
@@ -2701,7 +2738,7 @@
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B8" s="1">
         <v>5</v>
@@ -2728,8 +2765,8 @@
       <c r="V8" s="1"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>25</v>
+      <c r="A9" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="B9" s="1">
         <v>13</v>
@@ -2745,12 +2782,22 @@
       <c r="K9" s="1">
         <v>2</v>
       </c>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
+      <c r="L9" s="1">
+        <v>2</v>
+      </c>
+      <c r="M9" s="1">
+        <v>3</v>
+      </c>
+      <c r="N9" s="1">
+        <v>2</v>
+      </c>
       <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
+      <c r="P9" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>4</v>
+      </c>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
@@ -2759,7 +2806,7 @@
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B10" s="1">
         <v>8</v>
@@ -2778,7 +2825,9 @@
       <c r="L10" s="1">
         <v>2</v>
       </c>
-      <c r="M10" s="1"/>
+      <c r="M10" s="1">
+        <v>1</v>
+      </c>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
@@ -2791,10 +2840,10 @@
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B11" s="1">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -2809,7 +2858,9 @@
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
+      <c r="P11" s="1">
+        <v>3</v>
+      </c>
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
@@ -2819,7 +2870,7 @@
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12" s="1">
         <v>3</v>
@@ -2835,7 +2886,9 @@
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
+      <c r="N12" s="1">
+        <v>2</v>
+      </c>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
@@ -2847,7 +2900,7 @@
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B13" s="1">
         <v>1</v>
@@ -2877,7 +2930,7 @@
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B14" s="1">
         <v>1</v>
@@ -2907,7 +2960,7 @@
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B15" s="1">
         <v>3</v>
@@ -2939,7 +2992,7 @@
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B16" s="1">
         <v>8</v>
@@ -2958,11 +3011,19 @@
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
+      <c r="M16" s="1">
+        <v>1</v>
+      </c>
       <c r="N16" s="1"/>
-      <c r="O16" s="1"/>
-      <c r="P16" s="1"/>
-      <c r="Q16" s="1"/>
+      <c r="O16" s="1">
+        <v>2</v>
+      </c>
+      <c r="P16" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="1">
+        <v>1</v>
+      </c>
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
       <c r="T16" s="1"/>
@@ -2970,8 +3031,12 @@
       <c r="V16" s="1"/>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="1"/>
+      <c r="A17" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="1">
+        <v>3</v>
+      </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -2994,8 +3059,12 @@
       <c r="V17" s="1"/>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
+      <c r="A18" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="1">
+        <v>5</v>
+      </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -3018,8 +3087,12 @@
       <c r="V18" s="1"/>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
+      <c r="A19" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="1">
+        <v>3</v>
+      </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -3067,7 +3140,7 @@
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B21" s="1">
         <v>5</v>
@@ -3097,7 +3170,7 @@
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B22" s="1">
         <v>3</v>
@@ -3129,7 +3202,7 @@
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B23" s="1">
         <v>8</v>
@@ -3159,7 +3232,7 @@
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B24" s="1">
         <v>8</v>
@@ -3201,87 +3274,87 @@
       </c>
       <c r="B25" s="4">
         <f>SUM(B2:B24)</f>
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="C25" s="4">
         <f t="shared" ref="C25:V25" si="0">B25-SUM(C2:C24)</f>
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="D25" s="4">
         <f t="shared" si="0"/>
-        <v>98.5</v>
+        <v>104.5</v>
       </c>
       <c r="E25" s="4">
         <f t="shared" si="0"/>
-        <v>97.5</v>
+        <v>103.5</v>
       </c>
       <c r="F25" s="4">
         <f t="shared" si="0"/>
-        <v>92.5</v>
+        <v>98.5</v>
       </c>
       <c r="G25" s="4">
         <f t="shared" si="0"/>
-        <v>87.5</v>
+        <v>93.5</v>
       </c>
       <c r="H25" s="4">
         <f t="shared" si="0"/>
-        <v>85.5</v>
+        <v>91.5</v>
       </c>
       <c r="I25" s="4">
         <f t="shared" si="0"/>
-        <v>82.5</v>
+        <v>88.5</v>
       </c>
       <c r="J25" s="4">
         <f t="shared" si="0"/>
-        <v>77.5</v>
+        <v>81.5</v>
       </c>
       <c r="K25" s="4">
         <f t="shared" si="0"/>
-        <v>70.5</v>
+        <v>74.5</v>
       </c>
       <c r="L25" s="4">
         <f t="shared" si="0"/>
-        <v>64.5</v>
+        <v>66.5</v>
       </c>
       <c r="M25" s="4">
         <f t="shared" si="0"/>
-        <v>63.5</v>
+        <v>55.5</v>
       </c>
       <c r="N25" s="4">
         <f t="shared" si="0"/>
-        <v>63.5</v>
+        <v>45.5</v>
       </c>
       <c r="O25" s="4">
         <f t="shared" si="0"/>
-        <v>63.5</v>
+        <v>43.5</v>
       </c>
       <c r="P25" s="4">
         <f t="shared" si="0"/>
-        <v>63.5</v>
+        <v>37.5</v>
       </c>
       <c r="Q25" s="4">
         <f t="shared" si="0"/>
-        <v>63.5</v>
+        <v>32.5</v>
       </c>
       <c r="R25" s="4">
         <f t="shared" si="0"/>
-        <v>63.5</v>
+        <v>32.5</v>
       </c>
       <c r="S25" s="4">
         <f t="shared" si="0"/>
-        <v>63.5</v>
+        <v>32.5</v>
       </c>
       <c r="T25" s="4">
         <f t="shared" si="0"/>
-        <v>63.5</v>
+        <v>32.5</v>
       </c>
       <c r="U25" s="4">
         <f t="shared" si="0"/>
-        <v>63.5</v>
+        <v>32.5</v>
       </c>
       <c r="V25" s="4">
         <f t="shared" si="0"/>
-        <v>63.5</v>
+        <v>32.5</v>
       </c>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
@@ -3289,83 +3362,83 @@
         <v>22</v>
       </c>
       <c r="B26" s="6">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="C26" s="6">
         <f>$B$26-(($B$26/20)*(COLUMN()-2))</f>
-        <v>98.8</v>
+        <v>104.5</v>
       </c>
       <c r="D26" s="6">
         <f t="shared" ref="D26:V26" si="1">$B$26-(($B$26/20)*(COLUMN()-2))</f>
-        <v>93.6</v>
+        <v>99</v>
       </c>
       <c r="E26" s="6">
         <f t="shared" si="1"/>
-        <v>88.4</v>
+        <v>93.5</v>
       </c>
       <c r="F26" s="6">
         <f t="shared" si="1"/>
-        <v>83.2</v>
+        <v>88</v>
       </c>
       <c r="G26" s="6">
         <f t="shared" si="1"/>
-        <v>78</v>
+        <v>82.5</v>
       </c>
       <c r="H26" s="6">
         <f t="shared" si="1"/>
-        <v>72.8</v>
+        <v>77</v>
       </c>
       <c r="I26" s="6">
         <f t="shared" si="1"/>
-        <v>67.599999999999994</v>
+        <v>71.5</v>
       </c>
       <c r="J26" s="6">
         <f t="shared" si="1"/>
-        <v>62.4</v>
+        <v>66</v>
       </c>
       <c r="K26" s="6">
         <f t="shared" si="1"/>
-        <v>57.199999999999996</v>
+        <v>60.5</v>
       </c>
       <c r="L26" s="6">
         <f t="shared" si="1"/>
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="M26" s="6">
         <f t="shared" si="1"/>
-        <v>46.8</v>
+        <v>49.5</v>
       </c>
       <c r="N26" s="6">
         <f t="shared" si="1"/>
-        <v>41.599999999999994</v>
+        <v>44</v>
       </c>
       <c r="O26" s="6">
         <f t="shared" si="1"/>
-        <v>36.399999999999991</v>
+        <v>38.5</v>
       </c>
       <c r="P26" s="6">
         <f t="shared" si="1"/>
-        <v>31.200000000000003</v>
+        <v>33</v>
       </c>
       <c r="Q26" s="6">
         <f t="shared" si="1"/>
-        <v>26</v>
+        <v>27.5</v>
       </c>
       <c r="R26" s="6">
         <f t="shared" si="1"/>
-        <v>20.799999999999997</v>
+        <v>22</v>
       </c>
       <c r="S26" s="6">
         <f t="shared" si="1"/>
-        <v>15.599999999999994</v>
+        <v>16.5</v>
       </c>
       <c r="T26" s="6">
         <f t="shared" si="1"/>
-        <v>10.399999999999991</v>
+        <v>11</v>
       </c>
       <c r="U26" s="6">
         <f t="shared" si="1"/>
-        <v>5.2000000000000028</v>
+        <v>5.5</v>
       </c>
       <c r="V26" s="6">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
DOCS - burn sprint 2
</commit_message>
<xml_diff>
--- a/DOCS/burn_sprint2.xlsx
+++ b/DOCS/burn_sprint2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\FATEC\sem2\API-2\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E447C590-9DC0-4D76-A09A-6ECC9DC9A69E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC66EE2A-812A-4275-A1C2-0B123D6285F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>Total de horas</t>
   </si>
@@ -111,9 +111,6 @@
     <t>S1 - Daniel</t>
   </si>
   <si>
-    <t>S4 - Caio</t>
-  </si>
-  <si>
     <t>S6 - Monteiro</t>
   </si>
   <si>
@@ -163,6 +160,18 @@
   </si>
   <si>
     <t>S0 - Git e docs</t>
+  </si>
+  <si>
+    <t>S4 - Rafael</t>
+  </si>
+  <si>
+    <t>S10 - Front</t>
+  </si>
+  <si>
+    <t>S11 - Caio</t>
+  </si>
+  <si>
+    <t>S12 - Front</t>
   </si>
 </sst>
 </file>
@@ -925,67 +934,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>106</c:v>
+                  <c:v>119</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>105</c:v>
+                  <c:v>118</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>113.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>109.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>104.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>100.5</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>96.5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>91.5</c:v>
-                </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
+                  <c:v>97.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>92.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>87.5</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>84.5</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>79.5</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>74.5</c:v>
-                </c:pt>
                 <c:pt idx="9">
-                  <c:v>72.5</c:v>
+                  <c:v>85.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>62.5</c:v>
+                  <c:v>71.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>54</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>54</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>54</c:v>
+                  <c:v>49.5</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>54</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>54</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>54</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>54</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>54</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>54</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>54</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1099,64 +1108,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>106</c:v>
+                  <c:v>119</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100.7</c:v>
+                  <c:v>113.05</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>95.4</c:v>
+                  <c:v>107.1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>90.1</c:v>
+                  <c:v>101.15</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>84.8</c:v>
+                  <c:v>95.2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>79.5</c:v>
+                  <c:v>89.25</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>74.2</c:v>
+                  <c:v>83.3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>68.900000000000006</c:v>
+                  <c:v>77.349999999999994</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>63.6</c:v>
+                  <c:v>71.400000000000006</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>58.300000000000004</c:v>
+                  <c:v>65.449999999999989</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>53</c:v>
+                  <c:v>59.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>47.7</c:v>
+                  <c:v>53.55</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>42.400000000000006</c:v>
+                  <c:v>47.599999999999994</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>37.100000000000009</c:v>
+                  <c:v>41.649999999999991</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>31.799999999999997</c:v>
+                  <c:v>35.700000000000003</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>26.5</c:v>
+                  <c:v>29.75</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>21.200000000000003</c:v>
+                  <c:v>23.799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>15.900000000000006</c:v>
+                  <c:v>17.849999999999994</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>10.600000000000009</c:v>
+                  <c:v>11.899999999999991</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5.2999999999999972</c:v>
+                  <c:v>5.9500000000000028</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>0</c:v>
@@ -1568,67 +1577,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>106</c:v>
+                  <c:v>119</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>105</c:v>
+                  <c:v>118</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>113.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>109.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>104.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>100.5</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>96.5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>91.5</c:v>
-                </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
+                  <c:v>97.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>92.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>87.5</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>84.5</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>79.5</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>74.5</c:v>
-                </c:pt>
                 <c:pt idx="9">
-                  <c:v>72.5</c:v>
+                  <c:v>85.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>62.5</c:v>
+                  <c:v>71.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>54</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>54</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>54</c:v>
+                  <c:v>49.5</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>54</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>54</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>54</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>54</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>54</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>54</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>54</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1742,64 +1751,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>106</c:v>
+                  <c:v>119</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100.7</c:v>
+                  <c:v>113.05</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>95.4</c:v>
+                  <c:v>107.1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>90.1</c:v>
+                  <c:v>101.15</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>84.8</c:v>
+                  <c:v>95.2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>79.5</c:v>
+                  <c:v>89.25</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>74.2</c:v>
+                  <c:v>83.3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>68.900000000000006</c:v>
+                  <c:v>77.349999999999994</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>63.6</c:v>
+                  <c:v>71.400000000000006</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>58.300000000000004</c:v>
+                  <c:v>65.449999999999989</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>53</c:v>
+                  <c:v>59.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>47.7</c:v>
+                  <c:v>53.55</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>42.400000000000006</c:v>
+                  <c:v>47.599999999999994</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>37.100000000000009</c:v>
+                  <c:v>41.649999999999991</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>31.799999999999997</c:v>
+                  <c:v>35.700000000000003</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>26.5</c:v>
+                  <c:v>29.75</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>21.200000000000003</c:v>
+                  <c:v>23.799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>15.900000000000006</c:v>
+                  <c:v>17.849999999999994</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>10.600000000000009</c:v>
+                  <c:v>11.899999999999991</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5.2999999999999972</c:v>
+                  <c:v>5.9500000000000028</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>0</c:v>
@@ -2436,8 +2445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2553,7 +2562,7 @@
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3" s="1">
         <v>3</v>
@@ -2575,7 +2584,9 @@
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
+      <c r="P3" s="1">
+        <v>1</v>
+      </c>
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
@@ -2585,7 +2596,7 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" s="1">
         <v>3</v>
@@ -2603,7 +2614,9 @@
       <c r="M4" s="1">
         <v>1.5</v>
       </c>
-      <c r="N4" s="1"/>
+      <c r="N4" s="1">
+        <v>2</v>
+      </c>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
@@ -2615,7 +2628,7 @@
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" s="1">
         <v>3</v>
@@ -2634,8 +2647,12 @@
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
-      <c r="R5" s="1"/>
+      <c r="Q5" s="1">
+        <v>2</v>
+      </c>
+      <c r="R5" s="1">
+        <v>1</v>
+      </c>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
       <c r="U5" s="1"/>
@@ -2643,7 +2660,7 @@
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B6" s="1">
         <v>8</v>
@@ -2667,9 +2684,13 @@
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
+      <c r="P6" s="1">
+        <v>2</v>
+      </c>
       <c r="Q6" s="1"/>
-      <c r="R6" s="1"/>
+      <c r="R6" s="1">
+        <v>1</v>
+      </c>
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
       <c r="U6" s="1"/>
@@ -2677,7 +2698,7 @@
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B7" s="1">
         <v>8</v>
@@ -2691,7 +2712,9 @@
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
+      <c r="L7" s="1">
+        <v>2</v>
+      </c>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
@@ -2705,7 +2728,7 @@
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B8" s="1">
         <v>5</v>
@@ -2720,20 +2743,26 @@
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
+      <c r="M8" s="1">
+        <v>1</v>
+      </c>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
-      <c r="P8" s="1"/>
+      <c r="P8" s="1">
+        <v>2</v>
+      </c>
       <c r="Q8" s="1"/>
-      <c r="R8" s="1"/>
+      <c r="R8" s="1">
+        <v>2</v>
+      </c>
       <c r="S8" s="1"/>
       <c r="T8" s="1"/>
       <c r="U8" s="1"/>
       <c r="V8" s="1"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>25</v>
+      <c r="A9" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="B9" s="1">
         <v>13</v>
@@ -2750,12 +2779,20 @@
         <v>2</v>
       </c>
       <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
+      <c r="M9" s="1">
+        <v>2</v>
+      </c>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
-      <c r="R9" s="1"/>
+      <c r="P9" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>2</v>
+      </c>
+      <c r="R9" s="1">
+        <v>2</v>
+      </c>
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
       <c r="U9" s="1"/>
@@ -2763,7 +2800,7 @@
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B10" s="1">
         <v>8</v>
@@ -2787,7 +2824,9 @@
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
-      <c r="R10" s="1"/>
+      <c r="R10" s="1">
+        <v>2</v>
+      </c>
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
       <c r="U10" s="1"/>
@@ -2795,7 +2834,7 @@
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B11" s="1">
         <v>8</v>
@@ -2812,8 +2851,12 @@
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
+      <c r="O11" s="1">
+        <v>6.5</v>
+      </c>
+      <c r="P11" s="1">
+        <v>1.5</v>
+      </c>
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
@@ -2823,7 +2866,7 @@
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12" s="1">
         <v>3</v>
@@ -2837,8 +2880,12 @@
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
+      <c r="L12" s="1">
+        <v>1</v>
+      </c>
+      <c r="M12" s="1">
+        <v>2</v>
+      </c>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
@@ -2851,7 +2898,7 @@
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B13" s="1">
         <v>1</v>
@@ -2881,7 +2928,7 @@
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B14" s="1">
         <v>1</v>
@@ -2911,7 +2958,7 @@
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B15" s="1">
         <v>3</v>
@@ -2943,7 +2990,7 @@
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B16" s="1">
         <v>13</v>
@@ -2969,17 +3016,25 @@
       </c>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
-      <c r="P16" s="1"/>
+      <c r="P16" s="1">
+        <v>1</v>
+      </c>
       <c r="Q16" s="1"/>
-      <c r="R16" s="1"/>
+      <c r="R16" s="1">
+        <v>2</v>
+      </c>
       <c r="S16" s="1"/>
       <c r="T16" s="1"/>
       <c r="U16" s="1"/>
       <c r="V16" s="1"/>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="1"/>
+      <c r="A17" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="1">
+        <v>5</v>
+      </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -2995,15 +3050,21 @@
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
-      <c r="R17" s="1"/>
+      <c r="R17" s="1">
+        <v>1</v>
+      </c>
       <c r="S17" s="1"/>
       <c r="T17" s="1"/>
       <c r="U17" s="1"/>
       <c r="V17" s="1"/>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
+      <c r="A18" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="1">
+        <v>3</v>
+      </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -3013,21 +3074,29 @@
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
+      <c r="L18" s="1">
+        <v>1</v>
+      </c>
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
-      <c r="R18" s="1"/>
+      <c r="R18" s="1">
+        <v>2</v>
+      </c>
       <c r="S18" s="1"/>
       <c r="T18" s="1"/>
       <c r="U18" s="1"/>
       <c r="V18" s="1"/>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
+      <c r="A19" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="1">
+        <v>5</v>
+      </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -3043,7 +3112,9 @@
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
-      <c r="R19" s="1"/>
+      <c r="R19" s="1">
+        <v>1</v>
+      </c>
       <c r="S19" s="1"/>
       <c r="T19" s="1"/>
       <c r="U19" s="1"/>
@@ -3075,7 +3146,7 @@
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B21" s="1">
         <v>5</v>
@@ -3105,7 +3176,7 @@
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B22" s="1">
         <v>3</v>
@@ -3137,7 +3208,7 @@
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B23" s="1">
         <v>5</v>
@@ -3169,7 +3240,7 @@
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B24" s="1">
         <v>8</v>
@@ -3211,87 +3282,87 @@
       </c>
       <c r="B25" s="4">
         <f>SUM(B2:B24)</f>
-        <v>106</v>
+        <v>119</v>
       </c>
       <c r="C25" s="4">
         <f t="shared" ref="C25:V25" si="0">B25-SUM(C2:C24)</f>
-        <v>105</v>
+        <v>118</v>
       </c>
       <c r="D25" s="4">
         <f t="shared" si="0"/>
-        <v>100.5</v>
+        <v>113.5</v>
       </c>
       <c r="E25" s="4">
         <f t="shared" si="0"/>
-        <v>96.5</v>
+        <v>109.5</v>
       </c>
       <c r="F25" s="4">
         <f t="shared" si="0"/>
-        <v>91.5</v>
+        <v>104.5</v>
       </c>
       <c r="G25" s="4">
         <f t="shared" si="0"/>
-        <v>87.5</v>
+        <v>100.5</v>
       </c>
       <c r="H25" s="4">
         <f t="shared" si="0"/>
-        <v>84.5</v>
+        <v>97.5</v>
       </c>
       <c r="I25" s="4">
         <f>H25-SUM(I2:I24)</f>
-        <v>79.5</v>
+        <v>92.5</v>
       </c>
       <c r="J25" s="4">
         <f t="shared" si="0"/>
-        <v>74.5</v>
+        <v>87.5</v>
       </c>
       <c r="K25" s="4">
         <f t="shared" si="0"/>
-        <v>72.5</v>
+        <v>85.5</v>
       </c>
       <c r="L25" s="4">
         <f>K25-SUM(L2:L24)</f>
-        <v>62.5</v>
+        <v>71.5</v>
       </c>
       <c r="M25" s="4">
         <f t="shared" si="0"/>
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="N25" s="4">
         <f t="shared" si="0"/>
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="O25" s="4">
         <f t="shared" si="0"/>
-        <v>54</v>
+        <v>49.5</v>
       </c>
       <c r="P25" s="4">
         <f t="shared" si="0"/>
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="Q25" s="4">
         <f t="shared" si="0"/>
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="R25" s="4">
         <f t="shared" si="0"/>
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="S25" s="4">
         <f t="shared" si="0"/>
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="T25" s="4">
         <f t="shared" si="0"/>
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="U25" s="4">
         <f t="shared" si="0"/>
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="V25" s="4">
         <f t="shared" si="0"/>
-        <v>54</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
@@ -3299,83 +3370,83 @@
         <v>22</v>
       </c>
       <c r="B26" s="6">
-        <v>106</v>
+        <v>119</v>
       </c>
       <c r="C26" s="6">
         <f>$B$26-(($B$26/20)*(COLUMN()-2))</f>
-        <v>100.7</v>
+        <v>113.05</v>
       </c>
       <c r="D26" s="6">
         <f t="shared" ref="D26:V26" si="1">$B$26-(($B$26/20)*(COLUMN()-2))</f>
-        <v>95.4</v>
+        <v>107.1</v>
       </c>
       <c r="E26" s="6">
         <f t="shared" si="1"/>
-        <v>90.1</v>
+        <v>101.15</v>
       </c>
       <c r="F26" s="6">
         <f t="shared" si="1"/>
-        <v>84.8</v>
+        <v>95.2</v>
       </c>
       <c r="G26" s="6">
         <f t="shared" si="1"/>
-        <v>79.5</v>
+        <v>89.25</v>
       </c>
       <c r="H26" s="6">
         <f t="shared" si="1"/>
-        <v>74.2</v>
+        <v>83.3</v>
       </c>
       <c r="I26" s="6">
         <f t="shared" si="1"/>
-        <v>68.900000000000006</v>
+        <v>77.349999999999994</v>
       </c>
       <c r="J26" s="6">
         <f t="shared" si="1"/>
-        <v>63.6</v>
+        <v>71.400000000000006</v>
       </c>
       <c r="K26" s="6">
         <f t="shared" si="1"/>
-        <v>58.300000000000004</v>
+        <v>65.449999999999989</v>
       </c>
       <c r="L26" s="6">
         <f t="shared" si="1"/>
-        <v>53</v>
+        <v>59.5</v>
       </c>
       <c r="M26" s="6">
         <f t="shared" si="1"/>
-        <v>47.7</v>
+        <v>53.55</v>
       </c>
       <c r="N26" s="6">
         <f t="shared" si="1"/>
-        <v>42.400000000000006</v>
+        <v>47.599999999999994</v>
       </c>
       <c r="O26" s="6">
         <f t="shared" si="1"/>
-        <v>37.100000000000009</v>
+        <v>41.649999999999991</v>
       </c>
       <c r="P26" s="6">
         <f t="shared" si="1"/>
-        <v>31.799999999999997</v>
+        <v>35.700000000000003</v>
       </c>
       <c r="Q26" s="6">
         <f t="shared" si="1"/>
-        <v>26.5</v>
+        <v>29.75</v>
       </c>
       <c r="R26" s="6">
         <f t="shared" si="1"/>
-        <v>21.200000000000003</v>
+        <v>23.799999999999997</v>
       </c>
       <c r="S26" s="6">
         <f t="shared" si="1"/>
-        <v>15.900000000000006</v>
+        <v>17.849999999999994</v>
       </c>
       <c r="T26" s="6">
         <f t="shared" si="1"/>
-        <v>10.600000000000009</v>
+        <v>11.899999999999991</v>
       </c>
       <c r="U26" s="6">
         <f t="shared" si="1"/>
-        <v>5.2999999999999972</v>
+        <v>5.9500000000000028</v>
       </c>
       <c r="V26" s="6">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
DOCS - burndown sprint 2
</commit_message>
<xml_diff>
--- a/DOCS/burn_sprint2.xlsx
+++ b/DOCS/burn_sprint2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\FATEC\sem2\API-2\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC66EE2A-812A-4275-A1C2-0B123D6285F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01EEC194-4282-4BBE-A6EA-AD99708F024D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>Total de horas</t>
   </si>
@@ -133,9 +133,6 @@
   </si>
   <si>
     <t>S3.1 - Front</t>
-  </si>
-  <si>
-    <t>S3.2 - Front</t>
   </si>
   <si>
     <t>S3.3 - Front</t>
@@ -934,67 +931,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>119</c:v>
+                  <c:v>111</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>118</c:v>
+                  <c:v>110</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>113.5</c:v>
+                  <c:v>105.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>109.5</c:v>
+                  <c:v>101.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>104.5</c:v>
+                  <c:v>96.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>100.5</c:v>
+                  <c:v>92.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>97.5</c:v>
+                  <c:v>89.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>92.5</c:v>
+                  <c:v>84.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>87.5</c:v>
+                  <c:v>79.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>85.5</c:v>
+                  <c:v>77.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>71.5</c:v>
+                  <c:v>65.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>58</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>56</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>49.5</c:v>
+                  <c:v>43.5</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>40</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>36</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>22</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>22</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>22</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>22</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>22</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1108,64 +1105,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>119</c:v>
+                  <c:v>111</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>113.05</c:v>
+                  <c:v>105.45</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>107.1</c:v>
+                  <c:v>99.9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>101.15</c:v>
+                  <c:v>94.35</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>95.2</c:v>
+                  <c:v>88.8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>89.25</c:v>
+                  <c:v>83.25</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>83.3</c:v>
+                  <c:v>77.7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>77.349999999999994</c:v>
+                  <c:v>72.150000000000006</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>71.400000000000006</c:v>
+                  <c:v>66.599999999999994</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>65.449999999999989</c:v>
+                  <c:v>61.050000000000004</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>59.5</c:v>
+                  <c:v>55.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>53.55</c:v>
+                  <c:v>49.95</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>47.599999999999994</c:v>
+                  <c:v>44.400000000000006</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>41.649999999999991</c:v>
+                  <c:v>38.850000000000009</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>35.700000000000003</c:v>
+                  <c:v>33.299999999999997</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>29.75</c:v>
+                  <c:v>27.75</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>23.799999999999997</c:v>
+                  <c:v>22.200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>17.849999999999994</c:v>
+                  <c:v>16.650000000000006</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>11.899999999999991</c:v>
+                  <c:v>11.100000000000009</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5.9500000000000028</c:v>
+                  <c:v>5.5499999999999972</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>0</c:v>
@@ -1577,67 +1574,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>119</c:v>
+                  <c:v>111</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>118</c:v>
+                  <c:v>110</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>113.5</c:v>
+                  <c:v>105.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>109.5</c:v>
+                  <c:v>101.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>104.5</c:v>
+                  <c:v>96.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>100.5</c:v>
+                  <c:v>92.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>97.5</c:v>
+                  <c:v>89.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>92.5</c:v>
+                  <c:v>84.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>87.5</c:v>
+                  <c:v>79.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>85.5</c:v>
+                  <c:v>77.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>71.5</c:v>
+                  <c:v>65.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>58</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>56</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>49.5</c:v>
+                  <c:v>43.5</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>40</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>36</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>22</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>22</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>22</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>22</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>22</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1751,64 +1748,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>119</c:v>
+                  <c:v>111</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>113.05</c:v>
+                  <c:v>105.45</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>107.1</c:v>
+                  <c:v>99.9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>101.15</c:v>
+                  <c:v>94.35</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>95.2</c:v>
+                  <c:v>88.8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>89.25</c:v>
+                  <c:v>83.25</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>83.3</c:v>
+                  <c:v>77.7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>77.349999999999994</c:v>
+                  <c:v>72.150000000000006</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>71.400000000000006</c:v>
+                  <c:v>66.599999999999994</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>65.449999999999989</c:v>
+                  <c:v>61.050000000000004</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>59.5</c:v>
+                  <c:v>55.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>53.55</c:v>
+                  <c:v>49.95</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>47.599999999999994</c:v>
+                  <c:v>44.400000000000006</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>41.649999999999991</c:v>
+                  <c:v>38.850000000000009</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>35.700000000000003</c:v>
+                  <c:v>33.299999999999997</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>29.75</c:v>
+                  <c:v>27.75</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>23.799999999999997</c:v>
+                  <c:v>22.200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>17.849999999999994</c:v>
+                  <c:v>16.650000000000006</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>11.899999999999991</c:v>
+                  <c:v>11.100000000000009</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5.9500000000000028</c:v>
+                  <c:v>5.5499999999999972</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>0</c:v>
@@ -2445,8 +2442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="106" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V31" sqref="V31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2697,12 +2694,8 @@
       <c r="V6" s="1"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" s="1">
-        <v>8</v>
-      </c>
+      <c r="A7" s="2"/>
+      <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -2712,9 +2705,7 @@
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
-      <c r="L7" s="1">
-        <v>2</v>
-      </c>
+      <c r="L7" s="1"/>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
@@ -2728,7 +2719,7 @@
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B8" s="1">
         <v>5</v>
@@ -2762,7 +2753,7 @@
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B9" s="1">
         <v>13</v>
@@ -2796,7 +2787,9 @@
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
       <c r="U9" s="1"/>
-      <c r="V9" s="1"/>
+      <c r="V9" s="1">
+        <v>4</v>
+      </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -2827,7 +2820,9 @@
       <c r="R10" s="1">
         <v>2</v>
       </c>
-      <c r="S10" s="1"/>
+      <c r="S10" s="1">
+        <v>2</v>
+      </c>
       <c r="T10" s="1"/>
       <c r="U10" s="1"/>
       <c r="V10" s="1"/>
@@ -2898,7 +2893,7 @@
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B13" s="1">
         <v>1</v>
@@ -2928,7 +2923,7 @@
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B14" s="1">
         <v>1</v>
@@ -2958,7 +2953,7 @@
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B15" s="1">
         <v>3</v>
@@ -2990,7 +2985,7 @@
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B16" s="1">
         <v>13</v>
@@ -3030,7 +3025,7 @@
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B17" s="1">
         <v>5</v>
@@ -3055,12 +3050,14 @@
       </c>
       <c r="S17" s="1"/>
       <c r="T17" s="1"/>
-      <c r="U17" s="1"/>
+      <c r="U17" s="1">
+        <v>3</v>
+      </c>
       <c r="V17" s="1"/>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B18" s="1">
         <v>3</v>
@@ -3092,7 +3089,7 @@
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B19" s="1">
         <v>5</v>
@@ -3117,7 +3114,9 @@
       </c>
       <c r="S19" s="1"/>
       <c r="T19" s="1"/>
-      <c r="U19" s="1"/>
+      <c r="U19" s="1">
+        <v>2.5</v>
+      </c>
       <c r="V19" s="1"/>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.25">
@@ -3146,7 +3145,7 @@
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B21" s="1">
         <v>5</v>
@@ -3176,7 +3175,7 @@
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B22" s="1">
         <v>3</v>
@@ -3240,7 +3239,7 @@
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B24" s="1">
         <v>8</v>
@@ -3271,9 +3270,13 @@
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
-      <c r="S24" s="1"/>
+      <c r="S24" s="2">
+        <v>1.5</v>
+      </c>
       <c r="T24" s="1"/>
-      <c r="U24" s="1"/>
+      <c r="U24" s="1">
+        <v>3</v>
+      </c>
       <c r="V24" s="1"/>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
@@ -3282,87 +3285,87 @@
       </c>
       <c r="B25" s="4">
         <f>SUM(B2:B24)</f>
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="C25" s="4">
         <f t="shared" ref="C25:V25" si="0">B25-SUM(C2:C24)</f>
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="D25" s="4">
         <f t="shared" si="0"/>
-        <v>113.5</v>
+        <v>105.5</v>
       </c>
       <c r="E25" s="4">
         <f t="shared" si="0"/>
-        <v>109.5</v>
+        <v>101.5</v>
       </c>
       <c r="F25" s="4">
         <f t="shared" si="0"/>
-        <v>104.5</v>
+        <v>96.5</v>
       </c>
       <c r="G25" s="4">
         <f t="shared" si="0"/>
-        <v>100.5</v>
+        <v>92.5</v>
       </c>
       <c r="H25" s="4">
         <f t="shared" si="0"/>
-        <v>97.5</v>
+        <v>89.5</v>
       </c>
       <c r="I25" s="4">
         <f>H25-SUM(I2:I24)</f>
-        <v>92.5</v>
+        <v>84.5</v>
       </c>
       <c r="J25" s="4">
         <f t="shared" si="0"/>
-        <v>87.5</v>
+        <v>79.5</v>
       </c>
       <c r="K25" s="4">
         <f t="shared" si="0"/>
-        <v>85.5</v>
+        <v>77.5</v>
       </c>
       <c r="L25" s="4">
         <f>K25-SUM(L2:L24)</f>
-        <v>71.5</v>
+        <v>65.5</v>
       </c>
       <c r="M25" s="4">
         <f t="shared" si="0"/>
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="N25" s="4">
         <f t="shared" si="0"/>
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="O25" s="4">
         <f t="shared" si="0"/>
-        <v>49.5</v>
+        <v>43.5</v>
       </c>
       <c r="P25" s="4">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="Q25" s="4">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="R25" s="4">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="S25" s="4">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>12.5</v>
       </c>
       <c r="T25" s="4">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>12.5</v>
       </c>
       <c r="U25" s="4">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="V25" s="4">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
@@ -3370,83 +3373,83 @@
         <v>22</v>
       </c>
       <c r="B26" s="6">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="C26" s="6">
         <f>$B$26-(($B$26/20)*(COLUMN()-2))</f>
-        <v>113.05</v>
+        <v>105.45</v>
       </c>
       <c r="D26" s="6">
         <f t="shared" ref="D26:V26" si="1">$B$26-(($B$26/20)*(COLUMN()-2))</f>
-        <v>107.1</v>
+        <v>99.9</v>
       </c>
       <c r="E26" s="6">
         <f t="shared" si="1"/>
-        <v>101.15</v>
+        <v>94.35</v>
       </c>
       <c r="F26" s="6">
         <f t="shared" si="1"/>
-        <v>95.2</v>
+        <v>88.8</v>
       </c>
       <c r="G26" s="6">
         <f t="shared" si="1"/>
-        <v>89.25</v>
+        <v>83.25</v>
       </c>
       <c r="H26" s="6">
         <f t="shared" si="1"/>
-        <v>83.3</v>
+        <v>77.7</v>
       </c>
       <c r="I26" s="6">
         <f t="shared" si="1"/>
-        <v>77.349999999999994</v>
+        <v>72.150000000000006</v>
       </c>
       <c r="J26" s="6">
         <f t="shared" si="1"/>
-        <v>71.400000000000006</v>
+        <v>66.599999999999994</v>
       </c>
       <c r="K26" s="6">
         <f t="shared" si="1"/>
-        <v>65.449999999999989</v>
+        <v>61.050000000000004</v>
       </c>
       <c r="L26" s="6">
         <f t="shared" si="1"/>
-        <v>59.5</v>
+        <v>55.5</v>
       </c>
       <c r="M26" s="6">
         <f t="shared" si="1"/>
-        <v>53.55</v>
+        <v>49.95</v>
       </c>
       <c r="N26" s="6">
         <f t="shared" si="1"/>
-        <v>47.599999999999994</v>
+        <v>44.400000000000006</v>
       </c>
       <c r="O26" s="6">
         <f t="shared" si="1"/>
-        <v>41.649999999999991</v>
+        <v>38.850000000000009</v>
       </c>
       <c r="P26" s="6">
         <f t="shared" si="1"/>
-        <v>35.700000000000003</v>
+        <v>33.299999999999997</v>
       </c>
       <c r="Q26" s="6">
         <f t="shared" si="1"/>
-        <v>29.75</v>
+        <v>27.75</v>
       </c>
       <c r="R26" s="6">
         <f t="shared" si="1"/>
-        <v>23.799999999999997</v>
+        <v>22.200000000000003</v>
       </c>
       <c r="S26" s="6">
         <f t="shared" si="1"/>
-        <v>17.849999999999994</v>
+        <v>16.650000000000006</v>
       </c>
       <c r="T26" s="6">
         <f t="shared" si="1"/>
-        <v>11.899999999999991</v>
+        <v>11.100000000000009</v>
       </c>
       <c r="U26" s="6">
         <f t="shared" si="1"/>
-        <v>5.9500000000000028</v>
+        <v>5.5499999999999972</v>
       </c>
       <c r="V26" s="6">
         <f t="shared" si="1"/>

</xml_diff>